<commit_message>
Update vis plot scripts
</commit_message>
<xml_diff>
--- a/data/life_cycle_data.xlsx
+++ b/data/life_cycle_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoughton\Desktop\Github\saleos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DCD9E6-3111-4472-B51B-CF87D69E33D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63A46A5-A438-4FC7-ACF3-0361FA245F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3348" yWindow="1524" windowWidth="19908" windowHeight="14004" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
     <sheet name="Results Visualisation" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Final" sheetId="6" r:id="rId4"/>
+    <sheet name="Transpose" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="144">
   <si>
     <t>Impact category UUID</t>
   </si>
@@ -468,37 +469,7 @@
     <t>NF global</t>
   </si>
   <si>
-    <t>Falcon9</t>
-  </si>
-  <si>
-    <t>Ariane5</t>
-  </si>
-  <si>
-    <t>SoyuzFG</t>
-  </si>
-  <si>
-    <t>Launches</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>AIT</t>
-  </si>
-  <si>
-    <t>Propellant production</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>Launch campaign</t>
-  </si>
-  <si>
-    <t>system</t>
-  </si>
-  <si>
-    <t>stage</t>
+    <t>Constellation</t>
   </si>
 </sst>
 </file>
@@ -507,7 +478,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -529,6 +500,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -544,7 +516,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,8 +547,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -584,12 +562,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -601,71 +594,21 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -9340,7 +9283,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11379,9 +11322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11409,61 +11350,103 @@
     <col min="23" max="23" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14" t="s">
+      <c r="E1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="15" t="s">
+      <c r="L1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Z1" s="16" t="s">
+      <c r="S1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z1" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>77</v>
       </c>
@@ -11527,9 +11510,15 @@
       <c r="X2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="11"/>
+      <c r="Z2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -11843,7 +11832,7 @@
         <f>SUM(D5:J5)</f>
         <v>7545609269.0161886</v>
       </c>
-      <c r="AA5" s="35">
+      <c r="AA5" s="10">
         <f t="shared" si="1"/>
         <v>3587688581.0410113</v>
       </c>
@@ -11851,7 +11840,7 @@
         <f t="shared" si="2"/>
         <v>1363824795.1449556</v>
       </c>
-      <c r="AC5" s="34">
+      <c r="AC5" s="9">
         <f>AA5/1000000000</f>
         <v>3.5876885810410113</v>
       </c>
@@ -14259,17 +14248,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Z1:Z2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -14280,7 +14258,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14331,7 +14309,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -14375,7 +14353,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
@@ -14418,7 +14396,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5" t="s">
         <v>96</v>
       </c>
@@ -14492,7 +14470,7 @@
       <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -14536,7 +14514,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>95</v>
       </c>
@@ -14579,7 +14557,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>96</v>
       </c>
@@ -14651,7 +14629,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="21" t="s">
         <v>131</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -14687,7 +14665,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="5" t="s">
         <v>95</v>
       </c>
@@ -14722,7 +14700,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>96</v>
       </c>
@@ -14786,7 +14764,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="21" t="s">
         <v>132</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -14829,7 +14807,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>95</v>
       </c>
@@ -14871,7 +14849,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>96</v>
       </c>
@@ -14942,7 +14920,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -14978,7 +14956,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="5" t="s">
         <v>95</v>
       </c>
@@ -15013,7 +14991,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>96</v>
       </c>
@@ -15072,1071 +15050,1364 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EFF905-71F7-4E4C-A860-FECA9C454F58}">
+  <dimension ref="A1:AA7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="18" t="str">
+        <f>Results!C1</f>
+        <v>Reference unit</v>
+      </c>
+      <c r="D1" s="18" t="str">
+        <f>Results!D1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="E1" s="18" t="str">
+        <f>Results!E1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="F1" s="18" t="str">
+        <f>Results!F1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="G1" s="18" t="str">
+        <f>Results!G1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="H1" s="18" t="str">
+        <f>Results!H1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="I1" s="18" t="str">
+        <f>Results!I1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="J1" s="18" t="str">
+        <f>Results!J1</f>
+        <v>Kupier</v>
+      </c>
+      <c r="K1" s="18" t="str">
+        <f>Results!K1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="L1" s="18" t="str">
+        <f>Results!L1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="M1" s="18" t="str">
+        <f>Results!M1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="N1" s="18" t="str">
+        <f>Results!N1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="O1" s="18" t="str">
+        <f>Results!O1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="P1" s="18" t="str">
+        <f>Results!P1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="Q1" s="18" t="str">
+        <f>Results!Q1</f>
+        <v>Starlink</v>
+      </c>
+      <c r="R1" s="18" t="str">
+        <f>Results!R1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="S1" s="18" t="str">
+        <f>Results!S1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="T1" s="18" t="str">
+        <f>Results!T1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="U1" s="18" t="str">
+        <f>Results!U1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="V1" s="18" t="str">
+        <f>Results!V1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="W1" s="18" t="str">
+        <f>Results!W1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="X1" s="18" t="str">
+        <f>Results!X1</f>
+        <v>OneWeb</v>
+      </c>
+      <c r="Y1" s="18" t="str">
+        <f>Results!Z1</f>
+        <v>TOTAL Kupier</v>
+      </c>
+      <c r="Z1" s="18" t="str">
+        <f>Results!AA1</f>
+        <v>TOTAL Starlink</v>
+      </c>
+      <c r="AA1" s="18" t="str">
+        <f>Results!AB1</f>
+        <v>TOTAL OneWeb</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="str">
+        <f>Results!A2</f>
+        <v>Impact category UUID</v>
+      </c>
+      <c r="B2" s="18" t="str">
+        <f>Results!B2</f>
+        <v>Impact category</v>
+      </c>
+      <c r="C2" s="18" t="str">
+        <f>Results!C2</f>
+        <v>Reference unit</v>
+      </c>
+      <c r="D2" s="18" t="str">
+        <f>Results!D2</f>
+        <v>Ariane 5 Launches</v>
+      </c>
+      <c r="E2" s="18" t="str">
+        <f>Results!E2</f>
+        <v>Ariane 5 Production</v>
+      </c>
+      <c r="F2" s="18" t="str">
+        <f>Results!F2</f>
+        <v>Ariane 5 AIT</v>
+      </c>
+      <c r="G2" s="18" t="str">
+        <f>Results!G2</f>
+        <v>Ariane 5 Propellant Production</v>
+      </c>
+      <c r="H2" s="18" t="str">
+        <f>Results!H2</f>
+        <v>SCHD of Ariane 5 Propellant</v>
+      </c>
+      <c r="I2" s="18" t="str">
+        <f>Results!I2</f>
+        <v>Transportation of Ariane 5</v>
+      </c>
+      <c r="J2" s="18" t="str">
+        <f>Results!J2</f>
+        <v>Ariane 5 Launch Campaign</v>
+      </c>
+      <c r="K2" s="18" t="str">
+        <f>Results!K2</f>
+        <v>Falcon 9 Launches</v>
+      </c>
+      <c r="L2" s="18" t="str">
+        <f>Results!L2</f>
+        <v>Falcon 9 Production</v>
+      </c>
+      <c r="M2" s="18" t="str">
+        <f>Results!M2</f>
+        <v>Falcon 9 AIT</v>
+      </c>
+      <c r="N2" s="18" t="str">
+        <f>Results!N2</f>
+        <v>Falcon 9 Propellant Production</v>
+      </c>
+      <c r="O2" s="18" t="str">
+        <f>Results!O2</f>
+        <v>SCHD of Falcon 9 Propellant</v>
+      </c>
+      <c r="P2" s="18" t="str">
+        <f>Results!P2</f>
+        <v>Transportation of Falcon 9 by truck</v>
+      </c>
+      <c r="Q2" s="18" t="str">
+        <f>Results!Q2</f>
+        <v>Falcon 9 Launch Campaign</v>
+      </c>
+      <c r="R2" s="18" t="str">
+        <f>Results!R2</f>
+        <v>Soyuz-FG Launches</v>
+      </c>
+      <c r="S2" s="18" t="str">
+        <f>Results!S2</f>
+        <v>Soyuz-FG Production</v>
+      </c>
+      <c r="T2" s="18" t="str">
+        <f>Results!T2</f>
+        <v>Soyuz-FG AIT</v>
+      </c>
+      <c r="U2" s="18" t="str">
+        <f>Results!U2</f>
+        <v>Soyuz-FG Propellant Production</v>
+      </c>
+      <c r="V2" s="18" t="str">
+        <f>Results!V2</f>
+        <v>SCHD of Soyuz-FG Propellant</v>
+      </c>
+      <c r="W2" s="18" t="str">
+        <f>Results!W2</f>
+        <v>Transportation of Soyuz-FG by train</v>
+      </c>
+      <c r="X2" s="18" t="str">
+        <f>Results!X2</f>
+        <v>Soyuz-FG Launch Campaign</v>
+      </c>
+      <c r="Y2" s="18" t="str">
+        <f>Results!Z2</f>
+        <v>TOTAL Kupier</v>
+      </c>
+      <c r="Z2" s="18" t="str">
+        <f>Results!AA2</f>
+        <v>TOTAL Starlink</v>
+      </c>
+      <c r="AA2" s="18" t="str">
+        <f>Results!AB2</f>
+        <v>TOTAL OneWeb</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="str">
+        <f>Results!A5</f>
+        <v>305e2dd5-defb-4d89-8d38-d54a8ad9cdda</v>
+      </c>
+      <c r="B3" s="20" t="str">
+        <f>Results!B5</f>
+        <v>Climate Change - Global Warming Potential 100a</v>
+      </c>
+      <c r="C3" s="20" t="str">
+        <f>Results!C5</f>
+        <v>kg CO2 eq</v>
+      </c>
+      <c r="D3" s="20">
+        <f>Results!D5</f>
+        <v>5812740532.8000002</v>
+      </c>
+      <c r="E3" s="20">
+        <f>Results!E5</f>
+        <v>595012795.90014386</v>
+      </c>
+      <c r="F3" s="20">
+        <f>Results!F5</f>
+        <v>87278232.091468528</v>
+      </c>
+      <c r="G3" s="20">
+        <f>Results!G5</f>
+        <v>258836443.898379</v>
+      </c>
+      <c r="H3" s="20">
+        <f>Results!H5</f>
+        <v>485150868.1496706</v>
+      </c>
+      <c r="I3" s="20">
+        <f>Results!I5</f>
+        <v>596332.08846138336</v>
+      </c>
+      <c r="J3" s="20">
+        <f>Results!J5</f>
+        <v>305994064.08806497</v>
+      </c>
+      <c r="K3" s="20">
+        <f>Results!K5</f>
+        <v>1977942961.2047997</v>
+      </c>
+      <c r="L3" s="20">
+        <f>Results!L5</f>
+        <v>304401509.1212461</v>
+      </c>
+      <c r="M3" s="20">
+        <f>Results!M5</f>
+        <v>119603503.23645689</v>
+      </c>
+      <c r="N3" s="20">
+        <f>Results!N5</f>
+        <v>351111747.05649108</v>
+      </c>
+      <c r="O3" s="20">
+        <f>Results!O5</f>
+        <v>414029327.84313387</v>
+      </c>
+      <c r="P3" s="20">
+        <f>Results!P5</f>
+        <v>1274333.6433872997</v>
+      </c>
+      <c r="Q3" s="20">
+        <f>Results!Q5</f>
+        <v>419325198.93549639</v>
+      </c>
+      <c r="R3" s="20">
+        <f>Results!R5</f>
+        <v>240628743.792</v>
+      </c>
+      <c r="S3" s="20">
+        <f>Results!S5</f>
+        <v>893608259.62569189</v>
+      </c>
+      <c r="T3" s="20">
+        <f>Results!T5</f>
+        <v>32325271.144988347</v>
+      </c>
+      <c r="U3" s="20">
+        <f>Results!U5</f>
+        <v>19378203.988763895</v>
+      </c>
+      <c r="V3" s="20">
+        <f>Results!V5</f>
+        <v>64466609.669921778</v>
+      </c>
+      <c r="W3" s="20">
+        <f>Results!W5</f>
+        <v>86572.076158220516</v>
+      </c>
+      <c r="X3" s="20">
+        <f>Results!X5</f>
+        <v>113331134.84743147</v>
+      </c>
+      <c r="Y3" s="19">
+        <f>SUM(D3:J3)</f>
+        <v>7545609269.0161886</v>
+      </c>
+      <c r="Z3" s="19">
+        <f>SUM(K3:Q3)</f>
+        <v>3587688581.0410113</v>
+      </c>
+      <c r="AA3" s="19">
+        <f>SUM(R3:X3)</f>
+        <v>1363824795.1449556</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="str">
+        <f>Results!A16</f>
+        <v>5d5095a7-65cc-4657-8f3a-bd1c64f77b2b</v>
+      </c>
+      <c r="B4" s="20" t="str">
+        <f>Results!B16</f>
+        <v>Ozone Depletion - Ozone Depletion Potential (Steady State)</v>
+      </c>
+      <c r="C4" s="20" t="str">
+        <f>Results!C16</f>
+        <v>kg CFC-11 eq</v>
+      </c>
+      <c r="D4" s="20">
+        <f>Results!D16</f>
+        <v>11398514.4</v>
+      </c>
+      <c r="E4" s="20">
+        <f>Results!E16</f>
+        <v>40.269692768976711</v>
+      </c>
+      <c r="F4" s="20">
+        <f>Results!F16</f>
+        <v>8.4550659944016289</v>
+      </c>
+      <c r="G4" s="20">
+        <f>Results!G16</f>
+        <v>12.057808466225245</v>
+      </c>
+      <c r="H4" s="20">
+        <f>Results!H16</f>
+        <v>40.712090183799909</v>
+      </c>
+      <c r="I4" s="20">
+        <f>Results!I16</f>
+        <v>0.10221123460033958</v>
+      </c>
+      <c r="J4" s="20">
+        <f>Results!J16</f>
+        <v>42.005001854485108</v>
+      </c>
+      <c r="K4" s="20">
+        <f>Results!K16</f>
+        <v>2276780.94</v>
+      </c>
+      <c r="L4" s="20">
+        <f>Results!L16</f>
+        <v>20.533410038395193</v>
+      </c>
+      <c r="M4" s="20">
+        <f>Results!M16</f>
+        <v>11.586571918254084</v>
+      </c>
+      <c r="N4" s="20">
+        <f>Results!N16</f>
+        <v>40.468724318488675</v>
+      </c>
+      <c r="O4" s="20">
+        <f>Results!O16</f>
+        <v>36.957303083202042</v>
+      </c>
+      <c r="P4" s="20">
+        <f>Results!P16</f>
+        <v>0.26405299983326103</v>
+      </c>
+      <c r="Q4" s="20">
+        <f>Results!Q16</f>
+        <v>57.562409948738853</v>
+      </c>
+      <c r="R4" s="20">
+        <f>Results!R16</f>
+        <v>277445</v>
+      </c>
+      <c r="S4" s="20">
+        <f>Results!S16</f>
+        <v>62.2363545901934</v>
+      </c>
+      <c r="T4" s="20">
+        <f>Results!T16</f>
+        <v>3.1315059238524552</v>
+      </c>
+      <c r="U4" s="20">
+        <f>Results!U16</f>
+        <v>2.1999764600118605</v>
+      </c>
+      <c r="V4" s="20">
+        <f>Results!V16</f>
+        <v>5.7569720136658127</v>
+      </c>
+      <c r="W4" s="20">
+        <f>Results!W16</f>
+        <v>2.679102728956171E-2</v>
+      </c>
+      <c r="X4" s="20">
+        <f>Results!X16</f>
+        <v>15.557408094253745</v>
+      </c>
+      <c r="Y4" s="19">
+        <f>SUM(D4:J4)</f>
+        <v>11398658.001870502</v>
+      </c>
+      <c r="Z4" s="19">
+        <f>SUM(K4:Q4)</f>
+        <v>2276948.3124723062</v>
+      </c>
+      <c r="AA4" s="19">
+        <f>SUM(R4:X4)</f>
+        <v>277533.9090081093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="str">
+        <f>Results!A22</f>
+        <v>1bd12fe7-e558-4abd-86f1-e9ef7c3439b9</v>
+      </c>
+      <c r="B5" s="20" t="str">
+        <f>Results!B22</f>
+        <v xml:space="preserve">Resource Depletion - Mineral Resource Depletion Potential </v>
+      </c>
+      <c r="C5" s="20" t="str">
+        <f>Results!C22</f>
+        <v>kg Sb eq</v>
+      </c>
+      <c r="D5" s="20">
+        <f>Results!D22</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
+        <f>Results!E22</f>
+        <v>146865.1870889675</v>
+      </c>
+      <c r="F5" s="20">
+        <f>Results!F22</f>
+        <v>845.35187468534082</v>
+      </c>
+      <c r="G5" s="20">
+        <f>Results!G22</f>
+        <v>1868.2071180283422</v>
+      </c>
+      <c r="H5" s="20">
+        <f>Results!H22</f>
+        <v>27550.914375277629</v>
+      </c>
+      <c r="I5" s="20">
+        <f>Results!I22</f>
+        <v>10.51849323833415</v>
+      </c>
+      <c r="J5" s="20">
+        <f>Results!J22</f>
+        <v>1794.2045389180582</v>
+      </c>
+      <c r="K5" s="20">
+        <f>Results!K22</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="20">
+        <f>Results!L22</f>
+        <v>131966.94671489566</v>
+      </c>
+      <c r="M5" s="20">
+        <f>Results!M22</f>
+        <v>1158.4451616058375</v>
+      </c>
+      <c r="N5" s="20">
+        <f>Results!N22</f>
+        <v>2436.5707651715225</v>
+      </c>
+      <c r="O5" s="20">
+        <f>Results!O22</f>
+        <v>20554.015418601182</v>
+      </c>
+      <c r="P5" s="20">
+        <f>Results!P22</f>
+        <v>61.928501379508617</v>
+      </c>
+      <c r="Q5" s="20">
+        <f>Results!Q22</f>
+        <v>2458.7247385173391</v>
+      </c>
+      <c r="R5" s="20">
+        <f>Results!R22</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="20">
+        <f>Results!S22</f>
+        <v>249468.17206090401</v>
+      </c>
+      <c r="T5" s="20">
+        <f>Results!T22</f>
+        <v>313.09328692049661</v>
+      </c>
+      <c r="U5" s="20">
+        <f>Results!U22</f>
+        <v>134.32500979874089</v>
+      </c>
+      <c r="V5" s="20">
+        <f>Results!V22</f>
+        <v>3195.5139595683927</v>
+      </c>
+      <c r="W5" s="20">
+        <f>Results!W22</f>
+        <v>3.1698714888092043</v>
+      </c>
+      <c r="X5" s="20">
+        <f>Results!X22</f>
+        <v>664.52019959928077</v>
+      </c>
+      <c r="Y5" s="19">
+        <f>SUM(D5:J5)</f>
+        <v>178934.38348911522</v>
+      </c>
+      <c r="Z5" s="19">
+        <f>SUM(K5:Q5)</f>
+        <v>158636.63130017105</v>
+      </c>
+      <c r="AA5" s="19">
+        <f>SUM(R5:X5)</f>
+        <v>253778.79438827973</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="str">
+        <f>Results!A24</f>
+        <v>9a6e8ecd-bb0a-4204-ab5d-8686be10b6af</v>
+      </c>
+      <c r="B6" s="20" t="str">
+        <f>Results!B24</f>
+        <v>Toxicity - Freshwater Aquatic Ecotoxicity</v>
+      </c>
+      <c r="C6" s="20" t="str">
+        <f>Results!C24</f>
+        <v>PAF.m3.day</v>
+      </c>
+      <c r="D6" s="20">
+        <f>Results!D24</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="20">
+        <f>Results!E24</f>
+        <v>3765692023.6762009</v>
+      </c>
+      <c r="F6" s="20">
+        <f>Results!F24</f>
+        <v>415859129.60350496</v>
+      </c>
+      <c r="G6" s="20">
+        <f>Results!G24</f>
+        <v>924701310.17213857</v>
+      </c>
+      <c r="H6" s="20">
+        <f>Results!H24</f>
+        <v>3344674897.5176516</v>
+      </c>
+      <c r="I6" s="20">
+        <f>Results!I24</f>
+        <v>936461.40052167559</v>
+      </c>
+      <c r="J6" s="20">
+        <f>Results!J24</f>
+        <v>1008903428.0330663</v>
+      </c>
+      <c r="K6" s="20">
+        <f>Results!K24</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <f>Results!L24</f>
+        <v>1498766521.1906075</v>
+      </c>
+      <c r="M6" s="20">
+        <f>Results!M24</f>
+        <v>569881029.45665491</v>
+      </c>
+      <c r="N6" s="20">
+        <f>Results!N24</f>
+        <v>1131678388.6168551</v>
+      </c>
+      <c r="O6" s="20">
+        <f>Results!O24</f>
+        <v>2734227013.054121</v>
+      </c>
+      <c r="P6" s="20">
+        <f>Results!P24</f>
+        <v>3520269.0527360979</v>
+      </c>
+      <c r="Q6" s="20">
+        <f>Results!Q24</f>
+        <v>1382571364.3416095</v>
+      </c>
+      <c r="R6" s="20">
+        <f>Results!R24</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="20">
+        <f>Results!S24</f>
+        <v>5614078610.14048</v>
+      </c>
+      <c r="T6" s="20">
+        <f>Results!T24</f>
+        <v>154021899.85314998</v>
+      </c>
+      <c r="U6" s="20">
+        <f>Results!U24</f>
+        <v>62280861.958490282</v>
+      </c>
+      <c r="V6" s="20">
+        <f>Results!V24</f>
+        <v>425394806.89208257</v>
+      </c>
+      <c r="W6" s="20">
+        <f>Results!W24</f>
+        <v>458632.77336208906</v>
+      </c>
+      <c r="X6" s="20">
+        <f>Results!X24</f>
+        <v>373667936.30854309</v>
+      </c>
+      <c r="Y6" s="19">
+        <f>SUM(D6:J6)</f>
+        <v>9460767250.4030838</v>
+      </c>
+      <c r="Z6" s="19">
+        <f>SUM(K6:Q6)</f>
+        <v>7320644585.7125854</v>
+      </c>
+      <c r="AA6" s="19">
+        <f>SUM(R6:X6)</f>
+        <v>6629902747.9261084</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="str">
+        <f>Results!A25</f>
+        <v>5a9aec82-fca2-48bd-803d-66d103d777fb</v>
+      </c>
+      <c r="B7" s="20" t="str">
+        <f>Results!B25</f>
+        <v>Toxicity - Human Toxicity</v>
+      </c>
+      <c r="C7" s="20" t="str">
+        <f>Results!C25</f>
+        <v>cases</v>
+      </c>
+      <c r="D7" s="20">
+        <f>Results!D25</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <f>Results!E25</f>
+        <v>247.61081046303838</v>
+      </c>
+      <c r="F7" s="20">
+        <f>Results!F25</f>
+        <v>26.256644161334883</v>
+      </c>
+      <c r="G7" s="20">
+        <f>Results!G25</f>
+        <v>82.093704887785776</v>
+      </c>
+      <c r="H7" s="20">
+        <f>Results!H25</f>
+        <v>225.77985250222531</v>
+      </c>
+      <c r="I7" s="20">
+        <f>Results!I25</f>
+        <v>8.9312018866388954E-2</v>
+      </c>
+      <c r="J7" s="20">
+        <f>Results!J25</f>
+        <v>91.576513861203722</v>
+      </c>
+      <c r="K7" s="20">
+        <f>Results!K25</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="20">
+        <f>Results!L25</f>
+        <v>112.13279643924123</v>
+      </c>
+      <c r="M7" s="20">
+        <f>Results!M25</f>
+        <v>35.981327184051509</v>
+      </c>
+      <c r="N7" s="20">
+        <f>Results!N25</f>
+        <v>102.02586932806355</v>
+      </c>
+      <c r="O7" s="20">
+        <f>Results!O25</f>
+        <v>179.96259678193101</v>
+      </c>
+      <c r="P7" s="20">
+        <f>Results!P25</f>
+        <v>0.35273464827915968</v>
+      </c>
+      <c r="Q7" s="20">
+        <f>Results!Q25</f>
+        <v>125.4937412172051</v>
+      </c>
+      <c r="R7" s="20">
+        <f>Results!R25</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="20">
+        <f>Results!S25</f>
+        <v>382.72253795045799</v>
+      </c>
+      <c r="T7" s="20">
+        <f>Results!T25</f>
+        <v>9.7246830227166239</v>
+      </c>
+      <c r="U7" s="20">
+        <f>Results!U25</f>
+        <v>5.6281952025448847</v>
+      </c>
+      <c r="V7" s="20">
+        <f>Results!V25</f>
+        <v>27.99105677918498</v>
+      </c>
+      <c r="W7" s="20">
+        <f>Results!W25</f>
+        <v>5.1607458175010487E-2</v>
+      </c>
+      <c r="X7" s="20">
+        <f>Results!X25</f>
+        <v>33.917227356001376</v>
+      </c>
+      <c r="Y7" s="19">
+        <f>SUM(D7:J7)</f>
+        <v>673.40683789445438</v>
+      </c>
+      <c r="Z7" s="19">
+        <f>SUM(K7:Q7)</f>
+        <v>555.94906559877165</v>
+      </c>
+      <c r="AA7" s="19">
+        <f>SUM(R7:X7)</f>
+        <v>460.03530776908087</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445714A6-DB77-4E6D-8803-0121084C8619}">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:H26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="5" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="24" max="24" width="10.88671875" customWidth="1"/>
+    <col min="25" max="27" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f t="array" ref="A1:G24">TRANSPOSE(Final!A1:X7)</f>
+        <v>Constellation</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Impact category UUID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>305e2dd5-defb-4d89-8d38-d54a8ad9cdda</v>
+      </c>
+      <c r="D1" t="str">
+        <v>5d5095a7-65cc-4657-8f3a-bd1c64f77b2b</v>
+      </c>
+      <c r="E1" t="str">
+        <v>1bd12fe7-e558-4abd-86f1-e9ef7c3439b9</v>
+      </c>
+      <c r="F1" t="str">
+        <v>9a6e8ecd-bb0a-4204-ab5d-8686be10b6af</v>
+      </c>
+      <c r="G1" t="str">
+        <v>5a9aec82-fca2-48bd-803d-66d103d777fb</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" s="20" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="R2" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="S2" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z2" s="19" t="s">
-        <v>93</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <v>Constellation</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Impact category</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Climate Change - Global Warming Potential 100a</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Ozone Depletion - Ozone Depletion Potential (Steady State)</v>
+      </c>
+      <c r="E2" t="str">
+        <v xml:space="preserve">Resource Depletion - Mineral Resource Depletion Potential </v>
+      </c>
+      <c r="F2" t="str">
+        <v>Toxicity - Freshwater Aquatic Ecotoxicity</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Toxicity - Human Toxicity</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>Reference unit</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Reference unit</v>
+      </c>
+      <c r="C3" t="str">
+        <v>kg CO2 eq</v>
+      </c>
+      <c r="D3" t="str">
+        <v>kg CFC-11 eq</v>
+      </c>
+      <c r="E3" t="str">
+        <v>kg Sb eq</v>
+      </c>
+      <c r="F3" t="str">
+        <v>PAF.m3.day</v>
+      </c>
+      <c r="G3" t="str">
+        <v>cases</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Ariane 5 Launches</v>
+      </c>
+      <c r="C4">
         <v>5812740532.8000002</v>
       </c>
-      <c r="G3" s="2">
+      <c r="D4">
+        <v>11398514.4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Ariane 5 Production</v>
+      </c>
+      <c r="C5">
         <v>595012795.90014386</v>
       </c>
-      <c r="H3" s="2">
+      <c r="D5">
+        <v>40.269692768976711</v>
+      </c>
+      <c r="E5">
+        <v>146865.1870889675</v>
+      </c>
+      <c r="F5">
+        <v>3765692023.6762009</v>
+      </c>
+      <c r="G5">
+        <v>247.61081046303838</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Ariane 5 AIT</v>
+      </c>
+      <c r="C6">
         <v>87278232.091468528</v>
       </c>
-      <c r="I3" s="2">
+      <c r="D6">
+        <v>8.4550659944016289</v>
+      </c>
+      <c r="E6">
+        <v>845.35187468534082</v>
+      </c>
+      <c r="F6">
+        <v>415859129.60350496</v>
+      </c>
+      <c r="G6">
+        <v>26.256644161334883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Ariane 5 Propellant Production</v>
+      </c>
+      <c r="C7">
         <v>258836443.898379</v>
       </c>
-      <c r="J3" s="2">
+      <c r="D7">
+        <v>12.057808466225245</v>
+      </c>
+      <c r="E7">
+        <v>1868.2071180283422</v>
+      </c>
+      <c r="F7">
+        <v>924701310.17213857</v>
+      </c>
+      <c r="G7">
+        <v>82.093704887785776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B8" t="str">
+        <v>SCHD of Ariane 5 Propellant</v>
+      </c>
+      <c r="C8">
         <v>485150868.1496706</v>
       </c>
-      <c r="K3" s="2">
+      <c r="D8">
+        <v>40.712090183799909</v>
+      </c>
+      <c r="E8">
+        <v>27550.914375277629</v>
+      </c>
+      <c r="F8">
+        <v>3344674897.5176516</v>
+      </c>
+      <c r="G8">
+        <v>225.77985250222531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Transportation of Ariane 5</v>
+      </c>
+      <c r="C9">
         <v>596332.08846138336</v>
       </c>
-      <c r="L3" s="2">
+      <c r="D9">
+        <v>0.10221123460033958</v>
+      </c>
+      <c r="E9">
+        <v>10.51849323833415</v>
+      </c>
+      <c r="F9">
+        <v>936461.40052167559</v>
+      </c>
+      <c r="G9">
+        <v>8.9312018866388954E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <v>Kupier</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Ariane 5 Launch Campaign</v>
+      </c>
+      <c r="C10">
         <v>305994064.08806497</v>
       </c>
-      <c r="M3" s="2">
+      <c r="D10">
+        <v>42.005001854485108</v>
+      </c>
+      <c r="E10">
+        <v>1794.2045389180582</v>
+      </c>
+      <c r="F10">
+        <v>1008903428.0330663</v>
+      </c>
+      <c r="G10">
+        <v>91.576513861203722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Falcon 9 Launches</v>
+      </c>
+      <c r="C11">
         <v>1977942961.2047997</v>
       </c>
-      <c r="N3" s="2">
+      <c r="D11">
+        <v>2276780.94</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Falcon 9 Production</v>
+      </c>
+      <c r="C12">
         <v>304401509.1212461</v>
       </c>
-      <c r="O3" s="2">
+      <c r="D12">
+        <v>20.533410038395193</v>
+      </c>
+      <c r="E12">
+        <v>131966.94671489566</v>
+      </c>
+      <c r="F12">
+        <v>1498766521.1906075</v>
+      </c>
+      <c r="G12">
+        <v>112.13279643924123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Falcon 9 AIT</v>
+      </c>
+      <c r="C13">
         <v>119603503.23645689</v>
       </c>
-      <c r="P3" s="2">
+      <c r="D13">
+        <v>11.586571918254084</v>
+      </c>
+      <c r="E13">
+        <v>1158.4451616058375</v>
+      </c>
+      <c r="F13">
+        <v>569881029.45665491</v>
+      </c>
+      <c r="G13">
+        <v>35.981327184051509</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Falcon 9 Propellant Production</v>
+      </c>
+      <c r="C14">
         <v>351111747.05649108</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="D14">
+        <v>40.468724318488675</v>
+      </c>
+      <c r="E14">
+        <v>2436.5707651715225</v>
+      </c>
+      <c r="F14">
+        <v>1131678388.6168551</v>
+      </c>
+      <c r="G14">
+        <v>102.02586932806355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B15" t="str">
+        <v>SCHD of Falcon 9 Propellant</v>
+      </c>
+      <c r="C15">
         <v>414029327.84313387</v>
       </c>
-      <c r="R3" s="2">
+      <c r="D15">
+        <v>36.957303083202042</v>
+      </c>
+      <c r="E15">
+        <v>20554.015418601182</v>
+      </c>
+      <c r="F15">
+        <v>2734227013.054121</v>
+      </c>
+      <c r="G15">
+        <v>179.96259678193101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Transportation of Falcon 9 by truck</v>
+      </c>
+      <c r="C16">
         <v>1274333.6433872997</v>
       </c>
-      <c r="S3" s="2">
+      <c r="D16">
+        <v>0.26405299983326103</v>
+      </c>
+      <c r="E16">
+        <v>61.928501379508617</v>
+      </c>
+      <c r="F16">
+        <v>3520269.0527360979</v>
+      </c>
+      <c r="G16">
+        <v>0.35273464827915968</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <v>Starlink</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Falcon 9 Launch Campaign</v>
+      </c>
+      <c r="C17">
         <v>419325198.93549639</v>
       </c>
-      <c r="T3" s="2">
+      <c r="D17">
+        <v>57.562409948738853</v>
+      </c>
+      <c r="E17">
+        <v>2458.7247385173391</v>
+      </c>
+      <c r="F17">
+        <v>1382571364.3416095</v>
+      </c>
+      <c r="G17">
+        <v>125.4937412172051</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Soyuz-FG Launches</v>
+      </c>
+      <c r="C18">
         <v>240628743.792</v>
       </c>
-      <c r="U3" s="2">
+      <c r="D18">
+        <v>277445</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Soyuz-FG Production</v>
+      </c>
+      <c r="C19">
         <v>893608259.62569189</v>
       </c>
-      <c r="V3" s="2">
+      <c r="D19">
+        <v>62.2363545901934</v>
+      </c>
+      <c r="E19">
+        <v>249468.17206090401</v>
+      </c>
+      <c r="F19">
+        <v>5614078610.14048</v>
+      </c>
+      <c r="G19">
+        <v>382.72253795045799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Soyuz-FG AIT</v>
+      </c>
+      <c r="C20">
         <v>32325271.144988347</v>
       </c>
-      <c r="W3" s="2">
+      <c r="D20">
+        <v>3.1315059238524552</v>
+      </c>
+      <c r="E20">
+        <v>313.09328692049661</v>
+      </c>
+      <c r="F20">
+        <v>154021899.85314998</v>
+      </c>
+      <c r="G20">
+        <v>9.7246830227166239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Soyuz-FG Propellant Production</v>
+      </c>
+      <c r="C21">
         <v>19378203.988763895</v>
       </c>
-      <c r="X3" s="2">
+      <c r="D21">
+        <v>2.1999764600118605</v>
+      </c>
+      <c r="E21">
+        <v>134.32500979874089</v>
+      </c>
+      <c r="F21">
+        <v>62280861.958490282</v>
+      </c>
+      <c r="G21">
+        <v>5.6281952025448847</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B22" t="str">
+        <v>SCHD of Soyuz-FG Propellant</v>
+      </c>
+      <c r="C22">
         <v>64466609.669921778</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="D22">
+        <v>5.7569720136658127</v>
+      </c>
+      <c r="E22">
+        <v>3195.5139595683927</v>
+      </c>
+      <c r="F22">
+        <v>425394806.89208257</v>
+      </c>
+      <c r="G22">
+        <v>27.99105677918498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Transportation of Soyuz-FG by train</v>
+      </c>
+      <c r="C23">
         <v>86572.076158220516</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="D23">
+        <v>2.679102728956171E-2</v>
+      </c>
+      <c r="E23">
+        <v>3.1698714888092043</v>
+      </c>
+      <c r="F23">
+        <v>458632.77336208906</v>
+      </c>
+      <c r="G23">
+        <v>5.1607458175010487E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <v>OneWeb</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Soyuz-FG Launch Campaign</v>
+      </c>
+      <c r="C24">
         <v>113331134.84743147</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="2">
-        <v>11398514.4</v>
-      </c>
-      <c r="G4" s="2">
-        <v>40.269692768976711</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8.4550659944016289</v>
-      </c>
-      <c r="I4" s="2">
-        <v>12.057808466225245</v>
-      </c>
-      <c r="J4" s="2">
-        <v>40.712090183799909</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0.10221123460033958</v>
-      </c>
-      <c r="L4" s="2">
-        <v>42.005001854485108</v>
-      </c>
-      <c r="M4" s="2">
-        <v>2276780.94</v>
-      </c>
-      <c r="N4" s="2">
-        <v>20.533410038395193</v>
-      </c>
-      <c r="O4" s="2">
-        <v>11.586571918254084</v>
-      </c>
-      <c r="P4" s="2">
-        <v>40.468724318488675</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>36.957303083202042</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.26405299983326103</v>
-      </c>
-      <c r="S4" s="2">
-        <v>57.562409948738853</v>
-      </c>
-      <c r="T4" s="2">
-        <v>277445</v>
-      </c>
-      <c r="U4" s="2">
-        <v>62.2363545901934</v>
-      </c>
-      <c r="V4" s="2">
-        <v>3.1315059238524552</v>
-      </c>
-      <c r="W4" s="2">
-        <v>2.1999764600118605</v>
-      </c>
-      <c r="X4" s="2">
-        <v>5.7569720136658127</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>2.679102728956171E-2</v>
-      </c>
-      <c r="Z4" s="2">
+      <c r="D24">
         <v>15.557408094253745</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>146865.1870889675</v>
-      </c>
-      <c r="H5" s="2">
-        <v>845.35187468534082</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1868.2071180283422</v>
-      </c>
-      <c r="J5" s="2">
-        <v>27550.914375277629</v>
-      </c>
-      <c r="K5" s="2">
-        <v>10.51849323833415</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1794.2045389180582</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>131966.94671489566</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1158.4451616058375</v>
-      </c>
-      <c r="P5" s="2">
-        <v>2436.5707651715225</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>20554.015418601182</v>
-      </c>
-      <c r="R5" s="2">
-        <v>61.928501379508617</v>
-      </c>
-      <c r="S5" s="2">
-        <v>2458.7247385173391</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <v>249468.17206090401</v>
-      </c>
-      <c r="V5" s="2">
-        <v>313.09328692049661</v>
-      </c>
-      <c r="W5" s="2">
-        <v>134.32500979874089</v>
-      </c>
-      <c r="X5" s="2">
-        <v>3195.5139595683927</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>3.1698714888092043</v>
-      </c>
-      <c r="Z5" s="2">
+      <c r="E24">
         <v>664.52019959928077</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3765692023.6762009</v>
-      </c>
-      <c r="H6" s="2">
-        <v>415859129.60350496</v>
-      </c>
-      <c r="I6" s="2">
-        <v>924701310.17213857</v>
-      </c>
-      <c r="J6" s="2">
-        <v>3344674897.5176516</v>
-      </c>
-      <c r="K6" s="2">
-        <v>936461.40052167559</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1008903428.0330663</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1498766521.1906075</v>
-      </c>
-      <c r="O6" s="2">
-        <v>569881029.45665491</v>
-      </c>
-      <c r="P6" s="2">
-        <v>1131678388.6168551</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>2734227013.054121</v>
-      </c>
-      <c r="R6" s="2">
-        <v>3520269.0527360979</v>
-      </c>
-      <c r="S6" s="2">
-        <v>1382571364.3416095</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2">
-        <v>5614078610.14048</v>
-      </c>
-      <c r="V6" s="2">
-        <v>154021899.85314998</v>
-      </c>
-      <c r="W6" s="2">
-        <v>62280861.958490282</v>
-      </c>
-      <c r="X6" s="2">
-        <v>425394806.89208257</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>458632.77336208906</v>
-      </c>
-      <c r="Z6" s="2">
+      <c r="F24">
         <v>373667936.30854309</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>247.61081046303838</v>
-      </c>
-      <c r="H7" s="2">
-        <v>26.256644161334883</v>
-      </c>
-      <c r="I7" s="2">
-        <v>82.093704887785776</v>
-      </c>
-      <c r="J7" s="2">
-        <v>225.77985250222531</v>
-      </c>
-      <c r="K7" s="2">
-        <v>8.9312018866388954E-2</v>
-      </c>
-      <c r="L7" s="2">
-        <v>91.576513861203722</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>112.13279643924123</v>
-      </c>
-      <c r="O7" s="2">
-        <v>35.981327184051509</v>
-      </c>
-      <c r="P7" s="2">
-        <v>102.02586932806355</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>179.96259678193101</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.35273464827915968</v>
-      </c>
-      <c r="S7" s="2">
-        <v>125.4937412172051</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>382.72253795045799</v>
-      </c>
-      <c r="V7" s="2">
-        <v>9.7246830227166239</v>
-      </c>
-      <c r="W7" s="2">
-        <v>5.6281952025448847</v>
-      </c>
-      <c r="X7" s="2">
-        <v>27.99105677918498</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>5.1607458175010487E-2</v>
-      </c>
-      <c r="Z7" s="2">
+      <c r="G24">
         <v>33.917227356001376</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" s="28">
-        <v>5812740532.8000002</v>
-      </c>
-      <c r="E13" s="28">
-        <v>11398514.4</v>
-      </c>
-      <c r="F13" s="28">
-        <v>0</v>
-      </c>
-      <c r="G13" s="28">
-        <v>0</v>
-      </c>
-      <c r="H13" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="28">
-        <v>595012795.90014386</v>
-      </c>
-      <c r="E14" s="28">
-        <v>40.269692768976711</v>
-      </c>
-      <c r="F14" s="28">
-        <v>146865.1870889675</v>
-      </c>
-      <c r="G14" s="28">
-        <v>3765692023.6762009</v>
-      </c>
-      <c r="H14" s="28">
-        <v>247.61081046303838</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="28">
-        <v>87278232.091468528</v>
-      </c>
-      <c r="E15" s="28">
-        <v>8.4550659944016289</v>
-      </c>
-      <c r="F15" s="28">
-        <v>845.35187468534082</v>
-      </c>
-      <c r="G15" s="28">
-        <v>415859129.60350496</v>
-      </c>
-      <c r="H15" s="28">
-        <v>26.256644161334883</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="28">
-        <v>258836443.898379</v>
-      </c>
-      <c r="E16" s="28">
-        <v>12.057808466225245</v>
-      </c>
-      <c r="F16" s="28">
-        <v>1868.2071180283422</v>
-      </c>
-      <c r="G16" s="28">
-        <v>924701310.17213857</v>
-      </c>
-      <c r="H16" s="28">
-        <v>82.093704887785776</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D17" s="28">
-        <v>485150868.1496706</v>
-      </c>
-      <c r="E17" s="28">
-        <v>40.712090183799909</v>
-      </c>
-      <c r="F17" s="28">
-        <v>27550.914375277629</v>
-      </c>
-      <c r="G17" s="28">
-        <v>3344674897.5176516</v>
-      </c>
-      <c r="H17" s="28">
-        <v>225.77985250222531</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="28">
-        <v>596332.08846138336</v>
-      </c>
-      <c r="E18" s="28">
-        <v>0.10221123460033958</v>
-      </c>
-      <c r="F18" s="28">
-        <v>10.51849323833415</v>
-      </c>
-      <c r="G18" s="28">
-        <v>936461.40052167559</v>
-      </c>
-      <c r="H18" s="28">
-        <v>8.9312018866388954E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D19" s="28">
-        <v>305994064.08806497</v>
-      </c>
-      <c r="E19" s="28">
-        <v>42.005001854485108</v>
-      </c>
-      <c r="F19" s="28">
-        <v>1794.2045389180582</v>
-      </c>
-      <c r="G19" s="28">
-        <v>1008903428.0330663</v>
-      </c>
-      <c r="H19" s="28">
-        <v>91.576513861203722</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="28">
-        <v>1977942961.2047997</v>
-      </c>
-      <c r="E20" s="28">
-        <v>2276780.94</v>
-      </c>
-      <c r="F20" s="28">
-        <v>0</v>
-      </c>
-      <c r="G20" s="28">
-        <v>0</v>
-      </c>
-      <c r="H20" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="28">
-        <v>304401509.1212461</v>
-      </c>
-      <c r="E21" s="28">
-        <v>20.533410038395193</v>
-      </c>
-      <c r="F21" s="28">
-        <v>131966.94671489566</v>
-      </c>
-      <c r="G21" s="28">
-        <v>1498766521.1906075</v>
-      </c>
-      <c r="H21" s="28">
-        <v>112.13279643924123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="28">
-        <v>119603503.23645689</v>
-      </c>
-      <c r="E22" s="28">
-        <v>11.586571918254084</v>
-      </c>
-      <c r="F22" s="28">
-        <v>1158.4451616058375</v>
-      </c>
-      <c r="G22" s="28">
-        <v>569881029.45665491</v>
-      </c>
-      <c r="H22" s="28">
-        <v>35.981327184051509</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="29"/>
-      <c r="B23" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="28">
-        <v>351111747.05649108</v>
-      </c>
-      <c r="E23" s="28">
-        <v>40.468724318488675</v>
-      </c>
-      <c r="F23" s="28">
-        <v>2436.5707651715225</v>
-      </c>
-      <c r="G23" s="28">
-        <v>1131678388.6168551</v>
-      </c>
-      <c r="H23" s="28">
-        <v>102.02586932806355</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="28">
-        <v>414029327.84313387</v>
-      </c>
-      <c r="E24" s="28">
-        <v>36.957303083202042</v>
-      </c>
-      <c r="F24" s="28">
-        <v>20554.015418601182</v>
-      </c>
-      <c r="G24" s="28">
-        <v>2734227013.054121</v>
-      </c>
-      <c r="H24" s="28">
-        <v>179.96259678193101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D25" s="28">
-        <v>1274333.6433872997</v>
-      </c>
-      <c r="E25" s="28">
-        <v>0.26405299983326103</v>
-      </c>
-      <c r="F25" s="28">
-        <v>61.928501379508617</v>
-      </c>
-      <c r="G25" s="28">
-        <v>3520269.0527360979</v>
-      </c>
-      <c r="H25" s="28">
-        <v>0.35273464827915968</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="28">
-        <v>419325198.93549639</v>
-      </c>
-      <c r="E26" s="28">
-        <v>57.562409948738853</v>
-      </c>
-      <c r="F26" s="28">
-        <v>2458.7247385173391</v>
-      </c>
-      <c r="G26" s="28">
-        <v>1382571364.3416095</v>
-      </c>
-      <c r="H26" s="28">
-        <v>125.4937412172051</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="28">
-        <v>240628743.792</v>
-      </c>
-      <c r="E27" s="28">
-        <v>277445</v>
-      </c>
-      <c r="F27" s="28">
-        <v>0</v>
-      </c>
-      <c r="G27" s="28">
-        <v>0</v>
-      </c>
-      <c r="H27" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="28">
-        <v>893608259.62569189</v>
-      </c>
-      <c r="E28" s="28">
-        <v>62.2363545901934</v>
-      </c>
-      <c r="F28" s="28">
-        <v>249468.17206090401</v>
-      </c>
-      <c r="G28" s="28">
-        <v>5614078610.14048</v>
-      </c>
-      <c r="H28" s="28">
-        <v>382.72253795045799</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D29" s="28">
-        <v>32325271.144988347</v>
-      </c>
-      <c r="E29" s="28">
-        <v>3.1315059238524552</v>
-      </c>
-      <c r="F29" s="28">
-        <v>313.09328692049661</v>
-      </c>
-      <c r="G29" s="28">
-        <v>154021899.85314998</v>
-      </c>
-      <c r="H29" s="28">
-        <v>9.7246830227166239</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="28">
-        <v>19378203.988763895</v>
-      </c>
-      <c r="E30" s="28">
-        <v>2.1999764600118605</v>
-      </c>
-      <c r="F30" s="28">
-        <v>134.32500979874089</v>
-      </c>
-      <c r="G30" s="28">
-        <v>62280861.958490282</v>
-      </c>
-      <c r="H30" s="28">
-        <v>5.6281952025448847</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" s="28">
-        <v>64466609.669921778</v>
-      </c>
-      <c r="E31" s="28">
-        <v>5.7569720136658127</v>
-      </c>
-      <c r="F31" s="28">
-        <v>3195.5139595683927</v>
-      </c>
-      <c r="G31" s="28">
-        <v>425394806.89208257</v>
-      </c>
-      <c r="H31" s="28">
-        <v>27.99105677918498</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" s="28">
-        <v>86572.076158220516</v>
-      </c>
-      <c r="E32" s="28">
-        <v>2.679102728956171E-2</v>
-      </c>
-      <c r="F32" s="28">
-        <v>3.1698714888092043</v>
-      </c>
-      <c r="G32" s="28">
-        <v>458632.77336208906</v>
-      </c>
-      <c r="H32" s="28">
-        <v>5.1607458175010487E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="28">
-        <v>113331134.84743147</v>
-      </c>
-      <c r="E33" s="28">
-        <v>15.557408094253745</v>
-      </c>
-      <c r="F33" s="28">
-        <v>664.52019959928077</v>
-      </c>
-      <c r="G33" s="28">
-        <v>373667936.30854309</v>
-      </c>
-      <c r="H33" s="28">
-        <v>33.917227356001376</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D35" s="33">
-        <f>SUM(D20:D26)</f>
-        <v>3587688581.0410113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D36" s="34">
-        <f>D35/4425</f>
-        <v>810777.0804612455</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="T1:Z1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>